<commit_message>
after scraping 299 price sets from yahoo
</commit_message>
<xml_diff>
--- a/poc/asx300 - mapping scrapees.xlsx
+++ b/poc/asx300 - mapping scrapees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamish.macdonald/Documents/investing/scrapequity/poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DC93DCF-CB9F-774B-9398-CF3A8E0512B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A1559-34C5-FB4C-9958-F1FF8B53A7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{B39114B3-36C2-0A45-A414-6A35A328065A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="604">
   <si>
     <t>Code</t>
   </si>
@@ -2237,7 +2237,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2352,7 +2352,7 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2360,15 +2360,18 @@
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2376,7 +2379,7 @@
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2384,7 +2387,7 @@
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2392,7 +2395,7 @@
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>